<commit_message>
custom style radio buttons
</commit_message>
<xml_diff>
--- a/src/data/content/Website Content.xlsx
+++ b/src/data/content/Website Content.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="138">
   <si>
     <t>language</t>
   </si>
@@ -25,6 +25,18 @@
     <t>Tiếng Việt</t>
   </si>
   <si>
+    <t>languageCode</t>
+  </si>
+  <si>
+    <t>en</t>
+  </si>
+  <si>
+    <t>es</t>
+  </si>
+  <si>
+    <t>vi</t>
+  </si>
+  <si>
     <t>buttonHome</t>
   </si>
   <si>
@@ -395,6 +407,24 @@
   </si>
   <si>
     <t>Virtual Citizenship Workshop</t>
+  </si>
+  <si>
+    <t>errorMessageEmail</t>
+  </si>
+  <si>
+    <t>This field is required. Please use valid email format.</t>
+  </si>
+  <si>
+    <t>errorMessagePhone</t>
+  </si>
+  <si>
+    <t>This field is required. Please use the following format: ###-###-####</t>
+  </si>
+  <si>
+    <t>errorMessageZip</t>
+  </si>
+  <si>
+    <t>This field is required. Please use the following format: #####</t>
   </si>
 </sst>
 </file>
@@ -533,11 +563,11 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
+    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
@@ -785,242 +815,240 @@
       <c r="B2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B2,""en"",""es"")"),"Hogar")</f>
-        <v>Hogar</v>
-      </c>
-      <c r="D2" s="5" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B2,""en"",""vi"")"),"Trang Chủ")</f>
-        <v>Trang Chủ</v>
+      <c r="C2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C3" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B3,""en"",""es"")"),"Sobre")</f>
-        <v>Sobre</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B3,""en"",""es"")"),"Casa")</f>
+        <v>Casa</v>
       </c>
       <c r="D3" s="5" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B3,""en"",""vi"")"),"Trong khoảng")</f>
-        <v>Trong khoảng</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B3,""en"",""vi"")"),"Trang Chủ")</f>
+        <v>Trang Chủ</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C4" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B4,""en"",""es"")"),"CIIT fue diseñado por el Centro de Formación para el Empleo - Programa de Inmigración y Ciudadanía (CET-ICP)")</f>
-        <v>CIIT fue diseñado por el Centro de Formación para el Empleo - Programa de Inmigración y Ciudadanía (CET-ICP)</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B4,""en"",""es"")"),"Acerca de")</f>
+        <v>Acerca de</v>
       </c>
       <c r="D4" s="5" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B4,""en"",""vi"")"),"CIIT được thiết kế bởi Trung tâm Đào tạo Việc làm - Chương trình Di Trú &amp; Quốc tịch (CET-ICP)")</f>
-        <v>CIIT được thiết kế bởi Trung tâm Đào tạo Việc làm - Chương trình Di Trú &amp; Quốc tịch (CET-ICP)</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B4,""en"",""vi"")"),"Trong khoảng")</f>
+        <v>Trong khoảng</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C5" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B5,""en"",""es"")"),"CET-ICP es una organización sin ánimo de lucro 501C3")</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B5,""en"",""es"")"),"CIIT fue diseñado por el Centro de Formación para el Empleo - Programa de Inmigración y Ciudadanía (CET-ICP)")</f>
+        <v>CIIT fue diseñado por el Centro de Formación para el Empleo - Programa de Inmigración y Ciudadanía (CET-ICP)</v>
+      </c>
+      <c r="D5" s="5" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B5,""en"",""vi"")"),"CIIT được thiết kế bởi Trung tâm Đào tạo Việc làm - Chương trình Di Trú &amp; Quốc tịch (CET-ICP)")</f>
+        <v>CIIT được thiết kế bởi Trung tâm Đào tạo Việc làm - Chương trình Di Trú &amp; Quốc tịch (CET-ICP)</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="6" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B6,""en"",""es"")"),"CET-ICP es una organización sin ánimo de lucro 501C3")</f>
         <v>CET-ICP es una organización sin ánimo de lucro 501C3</v>
       </c>
-      <c r="D5" s="5" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B5,""en"",""vi"")"),"CET-ICP là một tổ chức phi lợi nhuận 501c3")</f>
+      <c r="D6" s="5" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B6,""en"",""vi"")"),"CET-ICP là một tổ chức phi lợi nhuận 501c3")</f>
         <v>CET-ICP là một tổ chức phi lợi nhuận 501c3</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="9" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B6,""en"",""es"")"),"Bienvenidos al Taller de Ciudadanía virtual")</f>
+    <row r="7">
+      <c r="A7" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="9" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B7,""en"",""es"")"),"Bienvenidos al Taller de Ciudadanía virtual")</f>
         <v>Bienvenidos al Taller de Ciudadanía virtual</v>
       </c>
-      <c r="D6" s="8" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B6,""en"",""vi"")"),"Chào mừng bạn đến Quốc tịch Hội thảo ảo")</f>
+      <c r="D7" s="8" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B7,""en"",""vi"")"),"Chào mừng bạn đến Quốc tịch Hội thảo ảo")</f>
         <v>Chào mừng bạn đến Quốc tịch Hội thảo ảo</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B7,""en"",""es"")"),"¿Cuál es el Taller de Ciudadanía virtual?")</f>
-        <v>¿Cuál es el Taller de Ciudadanía virtual?</v>
-      </c>
-      <c r="D7" s="5" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B7,""en"",""vi"")"),"Quốc tịch Hội thảo ảo là gì?")</f>
-        <v>Quốc tịch Hội thảo ảo là gì?</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="C8" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B8,""en"",""es"")"),"Este taller es una oportunidad para aprender más sobre el proceso de convertirse en un ciudadano de EE.UU., verificar su elegibilidad para solicitar la ciudadanía, y conectarse a la asistencia jurídica gratuita.")</f>
-        <v>Este taller es una oportunidad para aprender más sobre el proceso de convertirse en un ciudadano de EE.UU., verificar su elegibilidad para solicitar la ciudadanía, y conectarse a la asistencia jurídica gratuita.</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B8,""en"",""es"")"),"¿Cuál es el Taller de Ciudadanía virtual?")</f>
+        <v>¿Cuál es el Taller de Ciudadanía virtual?</v>
       </c>
       <c r="D8" s="5" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B8,""en"",""vi"")"),"Hội thảo này là một cơ hội để tìm hiểu thêm về quá trình để trở thành một công dân Hoa Kỳ, xác minh elegibility bạn để áp dụng cho công dân, và được kết nối với trợ giúp pháp lý miễn phí.")</f>
-        <v>Hội thảo này là một cơ hội để tìm hiểu thêm về quá trình để trở thành một công dân Hoa Kỳ, xác minh elegibility bạn để áp dụng cho công dân, và được kết nối với trợ giúp pháp lý miễn phí.</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B8,""en"",""vi"")"),"Quốc tịch Hội thảo ảo là gì?")</f>
+        <v>Quốc tịch Hội thảo ảo là gì?</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>21</v>
       </c>
       <c r="C9" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B9,""en"",""es"")"),"¿Quién puede participar?")</f>
-        <v>¿Quién puede participar?</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B9,""en"",""es"")"),"Este taller es una oportunidad para aprender más sobre el proceso de convertirse en un ciudadano de EE.UU., verificar su elegibilidad para solicitar la ciudadanía, y conectarse a la asistencia jurídica gratuita.")</f>
+        <v>Este taller es una oportunidad para aprender más sobre el proceso de convertirse en un ciudadano de EE.UU., verificar su elegibilidad para solicitar la ciudadanía, y conectarse a la asistencia jurídica gratuita.</v>
       </c>
       <c r="D9" s="5" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B9,""en"",""vi"")"),"Ai có thể tham gia?")</f>
-        <v>Ai có thể tham gia?</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B9,""en"",""vi"")"),"Hội thảo này là một cơ hội để tìm hiểu thêm về quá trình để trở thành một công dân Hoa Kỳ, xác minh elegibility bạn để áp dụng cho công dân, và được kết nối với trợ giúp pháp lý miễn phí.")</f>
+        <v>Hội thảo này là một cơ hội để tìm hiểu thêm về quá trình để trở thành một công dân Hoa Kỳ, xác minh elegibility bạn để áp dụng cho công dân, và được kết nối với trợ giúp pháp lý miễn phí.</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C10" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B10,""en"",""es"")"),"Dependiendo de la fecha en que usted se convirtió en un residente legal permanente, que puede o no ser capaz de participar en este taller.")</f>
-        <v>Dependiendo de la fecha en que usted se convirtió en un residente legal permanente, que puede o no ser capaz de participar en este taller.</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B10,""en"",""es"")"),"¿Quién puede participar?")</f>
+        <v>¿Quién puede participar?</v>
       </c>
       <c r="D10" s="5" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B10,""en"",""vi"")"),"Tùy thuộc vào ngày mà bạn trở thành một pháp thường trú, bạn có thể hoặc có thể không có khả năng tham gia hội thảo này.")</f>
-        <v>Tùy thuộc vào ngày mà bạn trở thành một pháp thường trú, bạn có thể hoặc có thể không có khả năng tham gia hội thảo này.</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B10,""en"",""vi"")"),"Ai có thể tham gia?")</f>
+        <v>Ai có thể tham gia?</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C11" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B11,""en"",""es"")"),"Pero no se preocupe, si usted no puede participar en este taller, es posible que pueda participar en futuros talleres.")</f>
-        <v>Pero no se preocupe, si usted no puede participar en este taller, es posible que pueda participar en futuros talleres.</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B11,""en"",""es"")"),"Dependiendo de la fecha en que usted se convirtió en un residente legal permanente, que puede o no ser capaz de participar en este taller.")</f>
+        <v>Dependiendo de la fecha en que usted se convirtió en un residente legal permanente, que puede o no ser capaz de participar en este taller.</v>
       </c>
       <c r="D11" s="5" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B11,""en"",""vi"")"),"Nhưng đừng lo lắng, nếu bạn không thể tham gia hội thảo này, bạn có thể tham gia vào các cuộc hội thảo tương lai.")</f>
-        <v>Nhưng đừng lo lắng, nếu bạn không thể tham gia hội thảo này, bạn có thể tham gia vào các cuộc hội thảo tương lai.</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B11,""en"",""vi"")"),"Tùy thuộc vào ngày mà bạn trở thành một pháp thường trú, bạn có thể hoặc có thể không có khả năng tham gia hội thảo này.")</f>
+        <v>Tùy thuộc vào ngày mà bạn trở thành một pháp thường trú, bạn có thể hoặc có thể không có khả năng tham gia hội thảo này.</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C12" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B12,""en"",""es"")"),"Vea si usted puede participar")</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B12,""en"",""es"")"),"Pero no se preocupe, si usted no puede participar en este taller, es posible que pueda participar en futuros talleres.")</f>
+        <v>Pero no se preocupe, si usted no puede participar en este taller, es posible que pueda participar en futuros talleres.</v>
+      </c>
+      <c r="D12" s="5" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B12,""en"",""vi"")"),"Nhưng đừng lo lắng, nếu bạn không thể tham gia hội thảo này, bạn có thể tham gia vào các cuộc hội thảo tương lai.")</f>
+        <v>Nhưng đừng lo lắng, nếu bạn không thể tham gia hội thảo này, bạn có thể tham gia vào các cuộc hội thảo tương lai.</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="6" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B13,""en"",""es"")"),"Vea si usted puede participar")</f>
         <v>Vea si usted puede participar</v>
       </c>
-      <c r="D12" s="5" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B12,""en"",""vi"")"),"Xem bạn có thể tham gia")</f>
+      <c r="D13" s="5" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B13,""en"",""vi"")"),"Xem bạn có thể tham gia")</f>
         <v>Xem bạn có thể tham gia</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" s="9" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B13,""en"",""es"")"),"Vamos a hacer seguro de que pueda participar en este taller")</f>
+    <row r="14">
+      <c r="A14" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="9" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B14,""en"",""es"")"),"Vamos a hacer seguro de que pueda participar en este taller")</f>
         <v>Vamos a hacer seguro de que pueda participar en este taller</v>
       </c>
-      <c r="D13" s="8" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B13,""en"",""vi"")"),"Hãy chắc chắn rằng bạn có thể tham gia hội thảo này")</f>
+      <c r="D14" s="8" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B14,""en"",""vi"")"),"Hãy chắc chắn rằng bạn có thể tham gia hội thảo này")</f>
         <v>Hãy chắc chắn rằng bạn có thể tham gia hội thảo này</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C14" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B14,""en"",""es"")"),"Contestar las preguntas 2-3 y averiguar si puede participar.")</f>
-        <v>Contestar las preguntas 2-3 y averiguar si puede participar.</v>
-      </c>
-      <c r="D14" s="5" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B14,""en"",""vi"")"),"Trả lời 2-3 câu hỏi và tìm hiểu xem bạn có thể tham gia.")</f>
-        <v>Trả lời 2-3 câu hỏi và tìm hiểu xem bạn có thể tham gia.</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C15" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B15,""en"",""es"")"),"Este campo es obligatorio")</f>
-        <v>Este campo es obligatorio</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B15,""en"",""es"")"),"Contestar las preguntas 2-3 y averiguar si puede participar.")</f>
+        <v>Contestar las preguntas 2-3 y averiguar si puede participar.</v>
       </c>
       <c r="D15" s="5" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B15,""en"",""vi"")"),"lĩnh vực này là cần thiết")</f>
-        <v>lĩnh vực này là cần thiết</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B15,""en"",""vi"")"),"Trả lời 2-3 câu hỏi và tìm hiểu xem bạn có thể tham gia.")</f>
+        <v>Trả lời 2-3 câu hỏi và tìm hiểu xem bạn có thể tham gia.</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" s="11">
-        <v>44256.0</v>
+        <v>34</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="C16" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B16,""en"",""es"")"),"01/03/2021")</f>
-        <v>01/03/2021</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B16,""en"",""es"")"),"Este campo es obligatorio")</f>
+        <v>Este campo es obligatorio</v>
       </c>
       <c r="D16" s="5" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B16,""en"",""vi"")"),"2021/03/01")</f>
-        <v>2021/03/01</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B16,""en"",""vi"")"),"lĩnh vực này là cần thiết")</f>
+        <v>lĩnh vực này là cần thiết</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="4" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B17" s="11">
         <v>44256.0</v>
@@ -1036,224 +1064,226 @@
     </row>
     <row r="18">
       <c r="A18" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>35</v>
+        <v>37</v>
+      </c>
+      <c r="B18" s="11">
+        <v>44256.0</v>
       </c>
       <c r="C18" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B18,""en"",""es"")"),"¡Lo lamentamos!")</f>
-        <v>¡Lo lamentamos!</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B18,""en"",""es"")"),"01/03/2021")</f>
+        <v>01/03/2021</v>
       </c>
       <c r="D18" s="5" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B18,""en"",""vi"")"),"Chúng tôi xin lỗi!")</f>
-        <v>Chúng tôi xin lỗi!</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B18,""en"",""vi"")"),"2021/03/01")</f>
+        <v>2021/03/01</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="4" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C19" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B19,""en"",""es"")"),"Con base en sus respuestas, no puede participar en este taller becuase:")</f>
-        <v>Con base en sus respuestas, no puede participar en este taller becuase:</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B19,""en"",""es"")"),"¡Lo lamentamos!")</f>
+        <v>¡Lo lamentamos!</v>
       </c>
       <c r="D19" s="5" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B19,""en"",""vi"")"),"Dựa trên phản ứng của bạn, bạn không thể tham gia hội thảo này bởi vì:")</f>
-        <v>Dựa trên phản ứng của bạn, bạn không thể tham gia hội thảo này bởi vì:</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B19,""en"",""vi"")"),"Chúng tôi xin lỗi!")</f>
+        <v>Chúng tôi xin lỗi!</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="4" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C20" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B20,""en"",""es"")"),"Usted ha sido un residente legal permanente durante menos de 2 años y 9 meses.")</f>
-        <v>Usted ha sido un residente legal permanente durante menos de 2 años y 9 meses.</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B20,""en"",""es"")"),"Con base en sus respuestas, no puede participar en este taller becuase:")</f>
+        <v>Con base en sus respuestas, no puede participar en este taller becuase:</v>
       </c>
       <c r="D20" s="5" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B20,""en"",""vi"")"),"Bạn đã là một thường trú nhân hợp pháp cho ít hơn 2 năm và 9 tháng.")</f>
-        <v>Bạn đã là một thường trú nhân hợp pháp cho ít hơn 2 năm và 9 tháng.</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B20,""en"",""vi"")"),"Dựa trên phản ứng của bạn, bạn không thể tham gia hội thảo này bởi vì:")</f>
+        <v>Dựa trên phản ứng của bạn, bạn không thể tham gia hội thảo này bởi vì:</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C21" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B21,""en"",""es"")"),"Usted ha sido un residente legal permanente durante menos de 4 años y 9 meses.")</f>
-        <v>Usted ha sido un residente legal permanente durante menos de 4 años y 9 meses.</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B21,""en"",""es"")"),"Usted ha sido un residente legal permanente durante menos de 2 años y 9 meses.")</f>
+        <v>Usted ha sido un residente legal permanente durante menos de 2 años y 9 meses.</v>
       </c>
       <c r="D21" s="5" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B21,""en"",""vi"")"),"Bạn đã là một thường trú nhân hợp pháp cho ít hơn 4 năm và 9 tháng.")</f>
-        <v>Bạn đã là một thường trú nhân hợp pháp cho ít hơn 4 năm và 9 tháng.</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B21,""en"",""vi"")"),"Bạn đã là một thường trú nhân hợp pháp cho ít hơn 2 năm và 9 tháng.")</f>
+        <v>Bạn đã là một thường trú nhân hợp pháp cho ít hơn 2 năm và 9 tháng.</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="4" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C22" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B22,""en"",""es"")"),"Salida")</f>
-        <v>Salida</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B22,""en"",""es"")"),"Usted ha sido un residente legal permanente durante menos de 4 años y 9 meses.")</f>
+        <v>Usted ha sido un residente legal permanente durante menos de 4 años y 9 meses.</v>
       </c>
       <c r="D22" s="5" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B22,""en"",""vi"")"),"Lối ra")</f>
-        <v>Lối ra</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B22,""en"",""vi"")"),"Bạn đã là một thường trú nhân hợp pháp cho ít hơn 4 năm và 9 tháng.")</f>
+        <v>Bạn đã là một thường trú nhân hợp pháp cho ít hơn 4 năm và 9 tháng.</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="4" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C23" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B23,""en"",""es"")"),"Enviar")</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B23,""en"",""es"")"),"Salida")</f>
+        <v>Salida</v>
+      </c>
+      <c r="D23" s="5" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B23,""en"",""vi"")"),"Lối ra")</f>
+        <v>Lối ra</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" s="6" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B24,""en"",""es"")"),"Enviar")</f>
         <v>Enviar</v>
       </c>
-      <c r="D23" s="5" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B23,""en"",""vi"")"),"Gửi đi")</f>
+      <c r="D24" s="5" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B24,""en"",""vi"")"),"Gửi đi")</f>
         <v>Gửi đi</v>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C24" s="9" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B24,""en"",""es"")"),"Bienvenidos al Taller de Ciudadanía virtual")</f>
+    <row r="25">
+      <c r="A25" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" s="9" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B25,""en"",""es"")"),"Bienvenidos al Taller de Ciudadanía virtual")</f>
         <v>Bienvenidos al Taller de Ciudadanía virtual</v>
       </c>
-      <c r="D24" s="8" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B24,""en"",""vi"")"),"Chào mừng bạn đến Quốc tịch Hội thảo ảo")</f>
+      <c r="D25" s="8" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B25,""en"",""vi"")"),"Chào mừng bạn đến Quốc tịch Hội thảo ảo")</f>
         <v>Chào mừng bạn đến Quốc tịch Hội thảo ảo</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C25" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B25,""en"",""es"")"),"¡Felicidades!")</f>
-        <v>¡Felicidades!</v>
-      </c>
-      <c r="D25" s="5" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B25,""en"",""vi"")"),"Xin chúc mừng!")</f>
-        <v>Xin chúc mừng!</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="4" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C26" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B26,""en"",""es"")"),"Con base en sus respuestas, se puede participar en este taller. Siga los pasos a continuación.")</f>
-        <v>Con base en sus respuestas, se puede participar en este taller. Siga los pasos a continuación.</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B26,""en"",""es"")"),"¡Felicidades!")</f>
+        <v>¡Felicidades!</v>
       </c>
       <c r="D26" s="5" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B26,""en"",""vi"")"),"Dựa trên câu trả lời của bạn, bạn có thể tham gia hội thảo này. Làm theo các bước dưới đây.")</f>
-        <v>Dựa trên câu trả lời của bạn, bạn có thể tham gia hội thảo này. Làm theo các bước dưới đây.</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B26,""en"",""vi"")"),"Xin chúc mừng!")</f>
+        <v>Xin chúc mừng!</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="4" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C27" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B27,""en"",""es"")"),"Ir a la Etapa 1")</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B27,""en"",""es"")"),"Con base en sus respuestas, se puede participar en este taller. Siga los pasos a continuación.")</f>
+        <v>Con base en sus respuestas, se puede participar en este taller. Siga los pasos a continuación.</v>
+      </c>
+      <c r="D27" s="5" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B27,""en"",""vi"")"),"Dựa trên câu trả lời của bạn, bạn có thể tham gia hội thảo này. Làm theo các bước dưới đây.")</f>
+        <v>Dựa trên câu trả lời của bạn, bạn có thể tham gia hội thảo này. Làm theo các bước dưới đây.</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C28" s="6" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B28,""en"",""es"")"),"Ir a la Etapa 1")</f>
         <v>Ir a la Etapa 1</v>
       </c>
-      <c r="D27" s="5" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B27,""en"",""vi"")"),"Tới Bước 1")</f>
+      <c r="D28" s="5" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B28,""en"",""vi"")"),"Tới Bước 1")</f>
         <v>Tới Bước 1</v>
       </c>
     </row>
-    <row r="28">
-      <c r="A28" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="B28" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="C28" s="9" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B28,""en"",""es"")"),"Paso 1")</f>
+    <row r="29">
+      <c r="A29" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C29" s="9" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B29,""en"",""es"")"),"Paso 1")</f>
         <v>Paso 1</v>
       </c>
-      <c r="D28" s="8" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B28,""en"",""vi"")"),"Bước 1")</f>
+      <c r="D29" s="8" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B29,""en"",""vi"")"),"Bước 1")</f>
         <v>Bước 1</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C29" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B29,""en"",""es"")"),"Video")</f>
-        <v>Video</v>
-      </c>
-      <c r="D29" s="5" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B29,""en"",""vi"")"),"Video")</f>
-        <v>Video</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C30" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B30,""en"",""es"")"),"Mira el vídeo de orientación de 15 minutos")</f>
-        <v>Mira el vídeo de orientación de 15 minutos</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B30,""en"",""es"")"),"Video")</f>
+        <v>Video</v>
       </c>
       <c r="D30" s="5" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B30,""en"",""vi"")"),"Xem hướng video dài 15 phút")</f>
-        <v>Xem hướng video dài 15 phút</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B30,""en"",""vi"")"),"Video")</f>
+        <v>Video</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="4" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="D31" s="5" t="s">
         <v>62</v>
+      </c>
+      <c r="C31" s="6" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B31,""en"",""es"")"),"Mira el vídeo de orientación de 15 minutos")</f>
+        <v>Mira el vídeo de orientación de 15 minutos</v>
+      </c>
+      <c r="D31" s="5" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B31,""en"",""vi"")"),"Xem hướng video dài 15 phút")</f>
+        <v>Xem hướng video dài 15 phút</v>
       </c>
     </row>
     <row r="32">
@@ -1263,546 +1293,588 @@
       <c r="B32" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C32" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B32,""en"",""es"")"),"Mira el vídeo de orientación proyecto nuevo ciudadano.")</f>
-        <v>Mira el vídeo de orientación proyecto nuevo ciudadano.</v>
-      </c>
-      <c r="D32" s="5" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B32,""en"",""vi"")"),"Xem video định hướng New Project Citizen.")</f>
-        <v>Xem video định hướng New Project Citizen.</v>
+      <c r="C32" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C33" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B33,""en"",""es"")"),"Sólo se tarda 15 minutos!")</f>
-        <v>Sólo se tarda 15 minutos!</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B33,""en"",""es"")"),"Mira el vídeo de orientación proyecto nuevo ciudadano.")</f>
+        <v>Mira el vídeo de orientación proyecto nuevo ciudadano.</v>
       </c>
       <c r="D33" s="5" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B33,""en"",""vi"")"),"Chỉ mất 15 phút!")</f>
-        <v>Chỉ mất 15 phút!</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B33,""en"",""vi"")"),"Xem video định hướng New Project Citizen.")</f>
+        <v>Xem video định hướng New Project Citizen.</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="4" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C34" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B34,""en"",""es"")"),"¡Gracias por ver!")</f>
-        <v>¡Gracias por ver!</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B34,""en"",""es"")"),"Sólo se tarda 15 minutos!")</f>
+        <v>Sólo se tarda 15 minutos!</v>
       </c>
       <c r="D34" s="5" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B34,""en"",""vi"")"),"Cảm ơn đã xem!")</f>
-        <v>Cảm ơn đã xem!</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B34,""en"",""vi"")"),"Chỉ mất 15 phút!")</f>
+        <v>Chỉ mất 15 phút!</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="4" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C35" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B35,""en"",""es"")"),"Ir a la Etapa 2")</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B35,""en"",""es"")"),"¡Gracias por ver!")</f>
+        <v>¡Gracias por ver!</v>
+      </c>
+      <c r="D35" s="5" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B35,""en"",""vi"")"),"Cảm ơn đã xem!")</f>
+        <v>Cảm ơn đã xem!</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C36" s="6" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B36,""en"",""es"")"),"Ir a la Etapa 2")</f>
         <v>Ir a la Etapa 2</v>
       </c>
-      <c r="D35" s="5" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B35,""en"",""vi"")"),"Tới Bước 2")</f>
+      <c r="D36" s="5" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B36,""en"",""vi"")"),"Tới Bước 2")</f>
         <v>Tới Bước 2</v>
       </c>
     </row>
-    <row r="36">
-      <c r="A36" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="B36" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="C36" s="9" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B36,""en"",""es"")"),"Paso 2")</f>
+    <row r="37">
+      <c r="A37" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C37" s="9" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B37,""en"",""es"")"),"Paso 2")</f>
         <v>Paso 2</v>
       </c>
-      <c r="D36" s="8" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B36,""en"",""vi"")"),"Bước 2")</f>
+      <c r="D37" s="8" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B37,""en"",""vi"")"),"Bước 2")</f>
         <v>Bước 2</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="C37" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B37,""en"",""es"")"),"Cuestionario")</f>
-        <v>Cuestionario</v>
-      </c>
-      <c r="D37" s="5" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B37,""en"",""vi"")"),"Bảng câu hỏi")</f>
-        <v>Bảng câu hỏi</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="4" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C38" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B38,""en"",""es"")"),"El cuestionario de selección")</f>
-        <v>El cuestionario de selección</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B38,""en"",""es"")"),"Cuestionario")</f>
+        <v>Cuestionario</v>
       </c>
       <c r="D38" s="5" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B38,""en"",""vi"")"),"Hoàn thành bảng câu hỏi sàng lọc")</f>
-        <v>Hoàn thành bảng câu hỏi sàng lọc</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B38,""en"",""vi"")"),"Bảng câu hỏi")</f>
+        <v>Bảng câu hỏi</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="4" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C39" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B39,""en"",""es"")"),"Se tarda aproximadamente 10 minutos")</f>
-        <v>Se tarda aproximadamente 10 minutos</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B39,""en"",""es"")"),"El cuestionario de selección")</f>
+        <v>El cuestionario de selección</v>
       </c>
       <c r="D39" s="5" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B39,""en"",""vi"")"),"Phải mất khoảng 10 phút")</f>
-        <v>Phải mất khoảng 10 phút</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B39,""en"",""vi"")"),"Hoàn thành bảng câu hỏi sàng lọc")</f>
+        <v>Hoàn thành bảng câu hỏi sàng lọc</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C40" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B40,""en"",""es"")"),"Responder a las preguntas 25-30")</f>
-        <v>Responder a las preguntas 25-30</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B40,""en"",""es"")"),"Se tarda aproximadamente 10 minutos")</f>
+        <v>Se tarda aproximadamente 10 minutos</v>
       </c>
       <c r="D40" s="5" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B40,""en"",""vi"")"),"Trả lời câu hỏi 25-30")</f>
-        <v>Trả lời câu hỏi 25-30</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B40,""en"",""vi"")"),"Phải mất khoảng 10 phút")</f>
+        <v>Phải mất khoảng 10 phút</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="4" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C41" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B41,""en"",""es"")"),"Es posible que tenga su Tarjeta Verde")</f>
-        <v>Es posible que tenga su Tarjeta Verde</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B41,""en"",""es"")"),"Responder a las preguntas 25-30")</f>
+        <v>Responder a las preguntas 25-30</v>
       </c>
       <c r="D41" s="5" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B41,""en"",""vi"")"),"Bạn có thể cần thẻ xanh của bạn")</f>
-        <v>Bạn có thể cần thẻ xanh của bạn</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B41,""en"",""vi"")"),"Trả lời câu hỏi 25-30")</f>
+        <v>Trả lời câu hỏi 25-30</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="4" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C42" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B42,""en"",""es"")"),"Sobre el cuestionario de selección")</f>
-        <v>Sobre el cuestionario de selección</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B42,""en"",""es"")"),"Es posible que tenga su Tarjeta Verde")</f>
+        <v>Es posible que tenga su Tarjeta Verde</v>
       </c>
       <c r="D42" s="5" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B42,""en"",""vi"")"),"Giới thiệu về câu hỏi sàng lọc")</f>
-        <v>Giới thiệu về câu hỏi sàng lọc</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B42,""en"",""vi"")"),"Bạn có thể cần thẻ xanh của bạn")</f>
+        <v>Bạn có thể cần thẻ xanh của bạn</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="4" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C43" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B43,""en"",""es"")"),"Toda su información será confidencial")</f>
-        <v>Toda su información será confidencial</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B43,""en"",""es"")"),"Sobre el cuestionario de selección")</f>
+        <v>Sobre el cuestionario de selección</v>
       </c>
       <c r="D43" s="5" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B43,""en"",""vi"")"),"Mọi thông tin của bạn sẽ được giữ bí mật")</f>
-        <v>Mọi thông tin của bạn sẽ được giữ bí mật</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B43,""en"",""vi"")"),"Giới thiệu về câu hỏi sàng lọc")</f>
+        <v>Giới thiệu về câu hỏi sàng lọc</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="4" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C44" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B44,""en"",""es"")"),"Por favor, conteste con sinceridad y lo mejor que puede recordar")</f>
-        <v>Por favor, conteste con sinceridad y lo mejor que puede recordar</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B44,""en"",""es"")"),"Toda su información será confidencial")</f>
+        <v>Toda su información será confidencial</v>
       </c>
       <c r="D44" s="5" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B44,""en"",""vi"")"),"Hãy trả lời trung thực và tốt nhất là khi bạn có thể nhớ")</f>
-        <v>Hãy trả lời trung thực và tốt nhất là khi bạn có thể nhớ</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B44,""en"",""vi"")"),"Mọi thông tin của bạn sẽ được giữ bí mật")</f>
+        <v>Mọi thông tin của bạn sẽ được giữ bí mật</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="4" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C45" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B45,""en"",""es"")"),"Por favor complete todas las preguntas en la medida de su capacidad")</f>
-        <v>Por favor complete todas las preguntas en la medida de su capacidad</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B45,""en"",""es"")"),"Por favor, conteste con sinceridad y lo mejor que puede recordar")</f>
+        <v>Por favor, conteste con sinceridad y lo mejor que puede recordar</v>
       </c>
       <c r="D45" s="5" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B45,""en"",""vi"")"),"Vui lòng điền TẤT CẢ các câu hỏi để hết khả năng của bạn")</f>
-        <v>Vui lòng điền TẤT CẢ các câu hỏi để hết khả năng của bạn</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B45,""en"",""vi"")"),"Hãy trả lời trung thực và tốt nhất là khi bạn có thể nhớ")</f>
+        <v>Hãy trả lời trung thực và tốt nhất là khi bạn có thể nhớ</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="B46" s="12" t="s">
-        <v>92</v>
+        <v>93</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>94</v>
       </c>
       <c r="C46" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B46,""en"",""es"")"),"Comience Cuestionario")</f>
-        <v>Comience Cuestionario</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B46,""en"",""es"")"),"Por favor complete todas las preguntas en la medida de su capacidad")</f>
+        <v>Por favor complete todas las preguntas en la medida de su capacidad</v>
       </c>
       <c r="D46" s="5" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B46,""en"",""vi"")"),"bắt đầu câu hỏi")</f>
-        <v>bắt đầu câu hỏi</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B46,""en"",""vi"")"),"Vui lòng điền TẤT CẢ các câu hỏi để hết khả năng của bạn")</f>
+        <v>Vui lòng điền TẤT CẢ các câu hỏi để hết khả năng của bạn</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="4" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C47" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B47,""en"",""es"")"),"Continuar")</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B47,""en"",""es"")"),"Comience Cuestionario")</f>
+        <v>Comience Cuestionario</v>
+      </c>
+      <c r="D47" s="5" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B47,""en"",""vi"")"),"bắt đầu câu hỏi")</f>
+        <v>bắt đầu câu hỏi</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C48" s="6" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B48,""en"",""es"")"),"Continuar")</f>
         <v>Continuar</v>
       </c>
-      <c r="D47" s="5" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B47,""en"",""vi"")"),"Tiếp tục")</f>
+      <c r="D48" s="5" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B48,""en"",""vi"")"),"Tiếp tục")</f>
         <v>Tiếp tục</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="B48" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="C48" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B48,""en"",""es"")"),"Enviar")</f>
-        <v>Enviar</v>
-      </c>
-      <c r="D48" s="5" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B48,""en"",""vi"")"),"Gửi đi")</f>
-        <v>Gửi đi</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="4" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>97</v>
+        <v>49</v>
       </c>
       <c r="C49" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B49,""en"",""es"")"),"Gracias por enviar el cuestionario de selección!")</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B49,""en"",""es"")"),"Enviar")</f>
+        <v>Enviar</v>
+      </c>
+      <c r="D49" s="5" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B49,""en"",""vi"")"),"Gửi đi")</f>
+        <v>Gửi đi</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C50" s="6" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B50,""en"",""es"")"),"Gracias por enviar el cuestionario de selección!")</f>
         <v>Gracias por enviar el cuestionario de selección!</v>
       </c>
-      <c r="D49" s="5" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B49,""en"",""vi"")"),"Cám ơn gửi bảng câu hỏi sàng lọc!")</f>
+      <c r="D50" s="5" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B50,""en"",""vi"")"),"Cám ơn gửi bảng câu hỏi sàng lọc!")</f>
         <v>Cám ơn gửi bảng câu hỏi sàng lọc!</v>
       </c>
     </row>
-    <row r="50">
-      <c r="A50" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="B50" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="C50" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B50,""en"",""es"")"),"Ir a la Etapa 3")</f>
+    <row r="51">
+      <c r="A51" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C51" s="6" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B51,""en"",""es"")"),"Ir a la Etapa 3")</f>
         <v>Ir a la Etapa 3</v>
       </c>
-      <c r="D50" s="5" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B50,""en"",""vi"")"),"Tới Bước 3")</f>
+      <c r="D51" s="5" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B51,""en"",""vi"")"),"Tới Bước 3")</f>
         <v>Tới Bước 3</v>
       </c>
     </row>
-    <row r="51">
-      <c r="A51" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="B51" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="C51" s="9" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B51,""en"",""es"")"),"Paso 3")</f>
+    <row r="52">
+      <c r="A52" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="B52" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="C52" s="9" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B52,""en"",""es"")"),"Paso 3")</f>
         <v>Paso 3</v>
       </c>
-      <c r="D51" s="8" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B51,""en"",""vi"")"),"Bước 3")</f>
+      <c r="D52" s="8" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B52,""en"",""vi"")"),"Bước 3")</f>
         <v>Bước 3</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="B52" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="C52" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B52,""en"",""es"")"),"Confirmación")</f>
-        <v>Confirmación</v>
-      </c>
-      <c r="D52" s="5" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B52,""en"",""vi"")"),"sự xác nhận")</f>
-        <v>sự xác nhận</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="4" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C53" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B53,""en"",""es"")"),"Descripción general de los próximos pasos para recibir asistencia jurídica gratuita")</f>
-        <v>Descripción general de los próximos pasos para recibir asistencia jurídica gratuita</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B53,""en"",""es"")"),"Confirmación")</f>
+        <v>Confirmación</v>
       </c>
       <c r="D53" s="5" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B53,""en"",""vi"")"),"Tổng quan về các bước tiếp theo để nhận trợ giúp pháp lý miễn phí")</f>
-        <v>Tổng quan về các bước tiếp theo để nhận trợ giúp pháp lý miễn phí</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B53,""en"",""vi"")"),"sự xác nhận")</f>
+        <v>sự xác nhận</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C54" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B54,""en"",""es"")"),"Enhorabuena, ha completado el taller!")</f>
-        <v>Enhorabuena, ha completado el taller!</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B54,""en"",""es"")"),"Descripción general de los próximos pasos para recibir asistencia jurídica gratuita")</f>
+        <v>Descripción general de los próximos pasos para recibir asistencia jurídica gratuita</v>
       </c>
       <c r="D54" s="5" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B54,""en"",""vi"")"),"Xin chúc mừng, bạn đã hoàn thành hội thảo!")</f>
-        <v>Xin chúc mừng, bạn đã hoàn thành hội thảo!</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B54,""en"",""vi"")"),"Tổng quan về các bước tiếp theo để nhận trợ giúp pháp lý miễn phí")</f>
+        <v>Tổng quan về các bước tiếp theo để nhận trợ giúp pháp lý miễn phí</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="4" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C55" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B55,""en"",""es"")"),"Hemos enviado una copia de esta página de confirmación al correo electrónico y / o teléfono que ha proporcionado en el cuestionario.")</f>
-        <v>Hemos enviado una copia de esta página de confirmación al correo electrónico y / o teléfono que ha proporcionado en el cuestionario.</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B55,""en"",""es"")"),"Enhorabuena, ha completado el taller!")</f>
+        <v>Enhorabuena, ha completado el taller!</v>
       </c>
       <c r="D55" s="5" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B55,""en"",""vi"")"),"Chúng tôi đã gửi một bản sao của trang xác nhận này cho email và / hoặc điện thoại mà bạn đã cung cấp trong bản câu hỏi.")</f>
-        <v>Chúng tôi đã gửi một bản sao của trang xác nhận này cho email và / hoặc điện thoại mà bạn đã cung cấp trong bản câu hỏi.</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B55,""en"",""vi"")"),"Xin chúc mừng, bạn đã hoàn thành hội thảo!")</f>
+        <v>Xin chúc mừng, bạn đã hoàn thành hội thảo!</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="4" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C56" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B56,""en"",""es"")"),"¿Que sigue?")</f>
-        <v>¿Que sigue?</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B56,""en"",""es"")"),"Hemos enviado una copia de esta página de confirmación al correo electrónico y / o teléfono que ha proporcionado en el cuestionario.")</f>
+        <v>Hemos enviado una copia de esta página de confirmación al correo electrónico y / o teléfono que ha proporcionado en el cuestionario.</v>
       </c>
       <c r="D56" s="5" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B56,""en"",""vi"")"),"Cái gì tiếp theo?")</f>
-        <v>Cái gì tiếp theo?</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B56,""en"",""vi"")"),"Chúng tôi đã gửi một bản sao của trang xác nhận này cho email và / hoặc điện thoại mà bạn đã cung cấp trong bản câu hỏi.")</f>
+        <v>Chúng tôi đã gửi một bản sao của trang xác nhận này cho email và / hoặc điện thoại mà bạn đã cung cấp trong bản câu hỏi.</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="4" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C57" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B57,""en"",""es"")"),"Si parece que usted es elegible para la ciudadanía en base a las respuestas que nos ha facilitado:")</f>
-        <v>Si parece que usted es elegible para la ciudadanía en base a las respuestas que nos ha facilitado:</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B57,""en"",""es"")"),"¿Que sigue?")</f>
+        <v>¿Que sigue?</v>
       </c>
       <c r="D57" s="5" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B57,""en"",""vi"")"),"Nếu nó xuất hiện rằng bạn có đủ điều kiện cho công dân dựa trên các câu trả lời mà bạn cung cấp:")</f>
-        <v>Nếu nó xuất hiện rằng bạn có đủ điều kiện cho công dân dựa trên các câu trả lời mà bạn cung cấp:</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B57,""en"",""vi"")"),"Cái gì tiếp theo?")</f>
+        <v>Cái gì tiếp theo?</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="4" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C58" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B58,""en"",""es"")"),"Un miembro del equipo de AEC-ICP se comunicará con usted dentro de las 48 horas por teléfono para una consulta de seguimiento GRATIS para verificar toda la información, el asesoramiento dar, y instuction.")</f>
-        <v>Un miembro del equipo de AEC-ICP se comunicará con usted dentro de las 48 horas por teléfono para una consulta de seguimiento GRATIS para verificar toda la información, el asesoramiento dar, y instuction.</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B58,""en"",""es"")"),"Si parece que usted es elegible para la ciudadanía en base a las respuestas que nos ha facilitado:")</f>
+        <v>Si parece que usted es elegible para la ciudadanía en base a las respuestas que nos ha facilitado:</v>
       </c>
       <c r="D58" s="5" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B58,""en"",""vi"")"),"thành viên trong nhóm Một CET-ICP sẽ liên lạc với bạn trong vòng 48 giờ qua điện thoại để được tư vấn theo dõi miễn phí để kiểm tra tất cả các thông tin, tư vấn Hãy cho, instuction.")</f>
-        <v>thành viên trong nhóm Một CET-ICP sẽ liên lạc với bạn trong vòng 48 giờ qua điện thoại để được tư vấn theo dõi miễn phí để kiểm tra tất cả các thông tin, tư vấn Hãy cho, instuction.</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B58,""en"",""vi"")"),"Nếu nó xuất hiện rằng bạn có đủ điều kiện cho công dân dựa trên các câu trả lời mà bạn cung cấp:")</f>
+        <v>Nếu nó xuất hiện rằng bạn có đủ điều kiện cho công dân dựa trên các câu trả lời mà bạn cung cấp:</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="4" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C59" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B59,""en"",""es"")"),"Si usted es elegible para solicitar, usted estará asistida por el Departamento de Justicia attourneys inmigración y representantes acreditados. La solicitud de ciudadanía assisstance será de forma gratuita, y toda la información se mantendrá confidencial.")</f>
-        <v>Si usted es elegible para solicitar, usted estará asistida por el Departamento de Justicia attourneys inmigración y representantes acreditados. La solicitud de ciudadanía assisstance será de forma gratuita, y toda la información se mantendrá confidencial.</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B59,""en"",""es"")"),"Un miembro del equipo de AEC-ICP se comunicará con usted dentro de las 48 horas por teléfono para una consulta de seguimiento GRATIS para verificar toda la información, el asesoramiento dar, y instuction.")</f>
+        <v>Un miembro del equipo de AEC-ICP se comunicará con usted dentro de las 48 horas por teléfono para una consulta de seguimiento GRATIS para verificar toda la información, el asesoramiento dar, y instuction.</v>
       </c>
       <c r="D59" s="5" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B59,""en"",""vi"")"),"Nếu bạn có đủ điều kiện để áp dụng, bạn sẽ được hỗ trợ bởi các attourneys nhập cư và DOJ công nhận đại diện. Việc áp dụng assisstance công dân sẽ được miễn phí phí, và tất cả các thông tin sẽ được giữ bí mật.")</f>
-        <v>Nếu bạn có đủ điều kiện để áp dụng, bạn sẽ được hỗ trợ bởi các attourneys nhập cư và DOJ công nhận đại diện. Việc áp dụng assisstance công dân sẽ được miễn phí phí, và tất cả các thông tin sẽ được giữ bí mật.</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B59,""en"",""vi"")"),"thành viên trong nhóm Một CET-ICP sẽ liên lạc với bạn trong vòng 48 giờ qua điện thoại để được tư vấn theo dõi miễn phí để kiểm tra tất cả các thông tin, tư vấn Hãy cho, instuction.")</f>
+        <v>thành viên trong nhóm Một CET-ICP sẽ liên lạc với bạn trong vòng 48 giờ qua điện thoại để được tư vấn theo dõi miễn phí để kiểm tra tất cả các thông tin, tư vấn Hãy cho, instuction.</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="4" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C60" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B60,""en"",""es"")"),"También recibirá recursos para ayudarle a estudiar para la entrevista de ciudadanía.")</f>
-        <v>También recibirá recursos para ayudarle a estudiar para la entrevista de ciudadanía.</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B60,""en"",""es"")"),"Si usted es elegible para solicitar, usted estará asistida por el Departamento de Justicia attourneys inmigración y representantes acreditados. La solicitud de ciudadanía assisstance será de forma gratuita, y toda la información se mantendrá confidencial.")</f>
+        <v>Si usted es elegible para solicitar, usted estará asistida por el Departamento de Justicia attourneys inmigración y representantes acreditados. La solicitud de ciudadanía assisstance será de forma gratuita, y toda la información se mantendrá confidencial.</v>
       </c>
       <c r="D60" s="5" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B60,""en"",""vi"")"),"Bạn cũng sẽ nhận được nguồn lực để giúp bạn học tập cho cuộc phỏng vấn công dân.")</f>
-        <v>Bạn cũng sẽ nhận được nguồn lực để giúp bạn học tập cho cuộc phỏng vấn công dân.</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B60,""en"",""vi"")"),"Nếu bạn có đủ điều kiện để áp dụng, bạn sẽ được hỗ trợ bởi các attourneys nhập cư và DOJ công nhận đại diện. Việc áp dụng assisstance công dân sẽ được miễn phí phí, và tất cả các thông tin sẽ được giữ bí mật.")</f>
+        <v>Nếu bạn có đủ điều kiện để áp dụng, bạn sẽ được hỗ trợ bởi các attourneys nhập cư và DOJ công nhận đại diện. Việc áp dụng assisstance công dân sẽ được miễn phí phí, và tất cả các thông tin sẽ được giữ bí mật.</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="4" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C61" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B61,""en"",""es"")"),"Si usted no es elegible para solicitar la ciudadanía en este momento, proporcionaremos una consulta libre inmigración en una fecha posterior.")</f>
-        <v>Si usted no es elegible para solicitar la ciudadanía en este momento, proporcionaremos una consulta libre inmigración en una fecha posterior.</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B61,""en"",""es"")"),"También recibirá recursos para ayudarle a estudiar para la entrevista de ciudadanía.")</f>
+        <v>También recibirá recursos para ayudarle a estudiar para la entrevista de ciudadanía.</v>
       </c>
       <c r="D61" s="5" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B61,""en"",""vi"")"),"Nếu bạn không đủ điều kiện để áp dụng cho công dân vào thời điểm này, chúng tôi sẽ cung cấp tư vấn di trú miễn phí vào một ngày sau đó.")</f>
-        <v>Nếu bạn không đủ điều kiện để áp dụng cho công dân vào thời điểm này, chúng tôi sẽ cung cấp tư vấn di trú miễn phí vào một ngày sau đó.</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B61,""en"",""vi"")"),"Bạn cũng sẽ nhận được nguồn lực để giúp bạn học tập cho cuộc phỏng vấn công dân.")</f>
+        <v>Bạn cũng sẽ nhận được nguồn lực để giúp bạn học tập cho cuộc phỏng vấn công dân.</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="4" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C62" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B62,""en"",""es"")"),"Nota: Debido al espacio limitado y COVID-19 mandato refugiarse en el lugar, no se puede garantizar que va a recibir los servicios. Gracias por su cooperación, paciencia y comprensión.")</f>
-        <v>Nota: Debido al espacio limitado y COVID-19 mandato refugiarse en el lugar, no se puede garantizar que va a recibir los servicios. Gracias por su cooperación, paciencia y comprensión.</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B62,""en"",""es"")"),"Si usted no es elegible para solicitar la ciudadanía en este momento, proporcionaremos una consulta libre inmigración en una fecha posterior.")</f>
+        <v>Si usted no es elegible para solicitar la ciudadanía en este momento, proporcionaremos una consulta libre inmigración en una fecha posterior.</v>
       </c>
       <c r="D62" s="5" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B62,""en"",""vi"")"),"Lưu ý: Do không gian hạn chế và COVID-19 nhiệm vụ nơi trú ẩn tại chỗ, chúng tôi không thể đảm bảo rằng bạn sẽ nhận được dịch vụ. Cảm ơn bạn đã hợp tác, kiên nhẫn và hiểu biết của bạn.")</f>
-        <v>Lưu ý: Do không gian hạn chế và COVID-19 nhiệm vụ nơi trú ẩn tại chỗ, chúng tôi không thể đảm bảo rằng bạn sẽ nhận được dịch vụ. Cảm ơn bạn đã hợp tác, kiên nhẫn và hiểu biết của bạn.</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B62,""en"",""vi"")"),"Nếu bạn không đủ điều kiện để áp dụng cho công dân vào thời điểm này, chúng tôi sẽ cung cấp tư vấn di trú miễn phí vào một ngày sau đó.")</f>
+        <v>Nếu bạn không đủ điều kiện để áp dụng cho công dân vào thời điểm này, chúng tôi sẽ cung cấp tư vấn di trú miễn phí vào một ngày sau đó.</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="4" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C63" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B63,""en"",""es"")"),"Si desea más información acerca de la inmigración, por favor visita")</f>
-        <v>Si desea más información acerca de la inmigración, por favor visita</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B63,""en"",""es"")"),"Nota: Debido al espacio limitado y COVID-19 mandato refugiarse en el lugar, no se puede garantizar que va a recibir los servicios. Gracias por su cooperación, paciencia y comprensión.")</f>
+        <v>Nota: Debido al espacio limitado y COVID-19 mandato refugiarse en el lugar, no se puede garantizar que va a recibir los servicios. Gracias por su cooperación, paciencia y comprensión.</v>
       </c>
       <c r="D63" s="5" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B63,""en"",""vi"")"),"Nếu bạn muốn biết thêm thông tin về di trú, hãy truy cập xin vui lòng")</f>
-        <v>Nếu bạn muốn biết thêm thông tin về di trú, hãy truy cập xin vui lòng</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B63,""en"",""vi"")"),"Lưu ý: Do không gian hạn chế và COVID-19 nhiệm vụ nơi trú ẩn tại chỗ, chúng tôi không thể đảm bảo rằng bạn sẽ nhận được dịch vụ. Cảm ơn bạn đã hợp tác, kiên nhẫn và hiểu biết của bạn.")</f>
+        <v>Lưu ý: Do không gian hạn chế và COVID-19 nhiệm vụ nơi trú ẩn tại chỗ, chúng tôi không thể đảm bảo rằng bạn sẽ nhận được dịch vụ. Cảm ơn bạn đã hợp tác, kiên nhẫn và hiểu biết của bạn.</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="4" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C64" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B64,""en"",""es"")"),"Taller de Ciudadanía virtual")</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B64,""en"",""es"")"),"Si desea más información acerca de la inmigración, por favor visita")</f>
+        <v>Si desea más información acerca de la inmigración, por favor visita</v>
+      </c>
+      <c r="D64" s="5" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B64,""en"",""vi"")"),"Nếu bạn muốn biết thêm thông tin về di trú, hãy truy cập xin vui lòng")</f>
+        <v>Nếu bạn muốn biết thêm thông tin về di trú, hãy truy cập xin vui lòng</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="C65" s="6" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B65,""en"",""es"")"),"Taller de Ciudadanía virtual")</f>
         <v>Taller de Ciudadanía virtual</v>
       </c>
-      <c r="D64" s="5" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B64,""en"",""vi"")"),"Quốc tịch Hội thảo ảo")</f>
+      <c r="D65" s="5" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B65,""en"",""vi"")"),"Quốc tịch Hội thảo ảo")</f>
         <v>Quốc tịch Hội thảo ảo</v>
       </c>
     </row>
-    <row r="65">
-      <c r="B65" s="14"/>
-      <c r="C65" s="14"/>
-      <c r="D65" s="14"/>
-    </row>
     <row r="66">
-      <c r="B66" s="14"/>
-      <c r="C66" s="14"/>
-      <c r="D66" s="14"/>
+      <c r="A66" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="B66" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="C66" s="6" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B66,""en"",""es"")"),"Este campo es requerido. Por favor utilice el formato de correo electrónico válida.")</f>
+        <v>Este campo es requerido. Por favor utilice el formato de correo electrónico válida.</v>
+      </c>
+      <c r="D66" s="5" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B66,""en"",""vi"")"),"Trường này là bắt buộc. Vui lòng sử dụng định dạng email hợp lệ.")</f>
+        <v>Trường này là bắt buộc. Vui lòng sử dụng định dạng email hợp lệ.</v>
+      </c>
     </row>
     <row r="67">
-      <c r="B67" s="14"/>
-      <c r="C67" s="14"/>
-      <c r="D67" s="14"/>
+      <c r="A67" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="B67" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="C67" s="6" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B67,""en"",""es"")"),"Este campo es requerido. Utilice el siguiente formato: ### - ### - ####")</f>
+        <v>Este campo es requerido. Utilice el siguiente formato: ### - ### - ####</v>
+      </c>
+      <c r="D67" s="5" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B67,""en"",""vi"")"),"Trường này là bắt buộc. Vui lòng sử dụng định dạng sau: ### - ### - ####")</f>
+        <v>Trường này là bắt buộc. Vui lòng sử dụng định dạng sau: ### - ### - ####</v>
+      </c>
     </row>
     <row r="68">
-      <c r="B68" s="14"/>
-      <c r="C68" s="14"/>
-      <c r="D68" s="14"/>
+      <c r="A68" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="B68" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="C68" s="6" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B68,""en"",""es"")"),"Este campo es requerido. Utilice el siguiente formato: #####")</f>
+        <v>Este campo es requerido. Utilice el siguiente formato: #####</v>
+      </c>
+      <c r="D68" s="5" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B68,""en"",""vi"")"),"Trường này là bắt buộc. Vui lòng sử dụng định dạng sau: #####")</f>
+        <v>Trường này là bắt buộc. Vui lòng sử dụng định dạng sau: #####</v>
+      </c>
     </row>
     <row r="69">
       <c r="B69" s="14"/>
@@ -6634,6 +6706,11 @@
       <c r="C1034" s="14"/>
       <c r="D1034" s="14"/>
     </row>
+    <row r="1035">
+      <c r="B1035" s="14"/>
+      <c r="C1035" s="14"/>
+      <c r="D1035" s="14"/>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>